<commit_message>
Further refactoring for better testing
</commit_message>
<xml_diff>
--- a/investment_tools/data/Company Financial Data/BHP/annual/stock_price_data.xlsx
+++ b/investment_tools/data/Company Financial Data/BHP/annual/stock_price_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>high</t>
   </si>
@@ -23,69 +23,6 @@
   </si>
   <si>
     <t>avg_close</t>
-  </si>
-  <si>
-    <t>index</t>
-  </si>
-  <si>
-    <t>BHP-FY-2003</t>
-  </si>
-  <si>
-    <t>BHP-FY-2004</t>
-  </si>
-  <si>
-    <t>BHP-FY-2005</t>
-  </si>
-  <si>
-    <t>BHP-FY-2006</t>
-  </si>
-  <si>
-    <t>BHP-FY-2007</t>
-  </si>
-  <si>
-    <t>BHP-FY-2008</t>
-  </si>
-  <si>
-    <t>BHP-FY-2009</t>
-  </si>
-  <si>
-    <t>BHP-FY-2010</t>
-  </si>
-  <si>
-    <t>BHP-FY-2011</t>
-  </si>
-  <si>
-    <t>BHP-FY-2012</t>
-  </si>
-  <si>
-    <t>BHP-FY-2013</t>
-  </si>
-  <si>
-    <t>BHP-FY-2014</t>
-  </si>
-  <si>
-    <t>BHP-FY-2015</t>
-  </si>
-  <si>
-    <t>BHP-FY-2016</t>
-  </si>
-  <si>
-    <t>BHP-FY-2017</t>
-  </si>
-  <si>
-    <t>BHP-FY-2018</t>
-  </si>
-  <si>
-    <t>BHP-FY-2019</t>
-  </si>
-  <si>
-    <t>BHP-FY-2020</t>
-  </si>
-  <si>
-    <t>BHP-FY-2021</t>
-  </si>
-  <si>
-    <t>BHP-FY-2022</t>
   </si>
 </sst>
 </file>
@@ -450,9 +387,6 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -464,8 +398,8 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
+      <c r="A2" s="1">
+        <v>0</v>
       </c>
       <c r="B2">
         <v>11.28456687927246</v>
@@ -478,8 +412,8 @@
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
+      <c r="A3" s="1">
+        <v>1</v>
       </c>
       <c r="B3">
         <v>17.930419921875</v>
@@ -492,8 +426,8 @@
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
+      <c r="A4" s="1">
+        <v>2</v>
       </c>
       <c r="B4">
         <v>27.66280174255371</v>
@@ -506,8 +440,8 @@
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
+      <c r="A5" s="1">
+        <v>3</v>
       </c>
       <c r="B5">
         <v>45.26315689086914</v>
@@ -520,8 +454,8 @@
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="1" t="s">
-        <v>8</v>
+      <c r="A6" s="1">
+        <v>4</v>
       </c>
       <c r="B6">
         <v>54.04103469848633</v>
@@ -534,8 +468,8 @@
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="1" t="s">
-        <v>9</v>
+      <c r="A7" s="1">
+        <v>5</v>
       </c>
       <c r="B7">
         <v>85.2899169921875</v>
@@ -548,8 +482,8 @@
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="1" t="s">
-        <v>10</v>
+      <c r="A8" s="1">
+        <v>6</v>
       </c>
       <c r="B8">
         <v>76.73506164550781</v>
@@ -562,8 +496,8 @@
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="1" t="s">
-        <v>11</v>
+      <c r="A9" s="1">
+        <v>7</v>
       </c>
       <c r="B9">
         <v>74.21944427490234</v>
@@ -576,8 +510,8 @@
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="1" t="s">
-        <v>12</v>
+      <c r="A10" s="1">
+        <v>8</v>
       </c>
       <c r="B10">
         <v>93.30062103271484</v>
@@ -590,8 +524,8 @@
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="1" t="s">
-        <v>13</v>
+      <c r="A11" s="1">
+        <v>9</v>
       </c>
       <c r="B11">
         <v>86.85994720458984</v>
@@ -604,8 +538,8 @@
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="1" t="s">
-        <v>14</v>
+      <c r="A12" s="1">
+        <v>10</v>
       </c>
       <c r="B12">
         <v>71.84656524658203</v>
@@ -618,8 +552,8 @@
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="1" t="s">
-        <v>15</v>
+      <c r="A13" s="1">
+        <v>11</v>
       </c>
       <c r="B13">
         <v>65.08474731445312</v>
@@ -632,8 +566,8 @@
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="1" t="s">
-        <v>16</v>
+      <c r="A14" s="1">
+        <v>12</v>
       </c>
       <c r="B14">
         <v>65.93220520019531</v>
@@ -646,8 +580,8 @@
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="1" t="s">
-        <v>17</v>
+      <c r="A15" s="1">
+        <v>13</v>
       </c>
       <c r="B15">
         <v>37.19892883300781</v>
@@ -660,8 +594,8 @@
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="1" t="s">
-        <v>18</v>
+      <c r="A16" s="1">
+        <v>14</v>
       </c>
       <c r="B16">
         <v>37.27921676635742</v>
@@ -674,8 +608,8 @@
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="1" t="s">
-        <v>19</v>
+      <c r="A17" s="1">
+        <v>15</v>
       </c>
       <c r="B17">
         <v>46.53880310058594</v>
@@ -688,8 +622,8 @@
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="1" t="s">
-        <v>20</v>
+      <c r="A18" s="1">
+        <v>16</v>
       </c>
       <c r="B18">
         <v>52.17662811279297</v>
@@ -702,8 +636,8 @@
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="1" t="s">
-        <v>21</v>
+      <c r="A19" s="1">
+        <v>17</v>
       </c>
       <c r="B19">
         <v>52.64942169189453</v>
@@ -716,8 +650,8 @@
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="1" t="s">
-        <v>22</v>
+      <c r="A20" s="1">
+        <v>18</v>
       </c>
       <c r="B20">
         <v>73.21141815185547</v>
@@ -730,8 +664,8 @@
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="1" t="s">
-        <v>23</v>
+      <c r="A21" s="1">
+        <v>19</v>
       </c>
       <c r="B21">
         <v>71.81088256835938</v>

</xml_diff>